<commit_message>
Terminado de pintar as partes do personagem feminino
</commit_message>
<xml_diff>
--- a/Sam's Adventures/Automatizador.xlsx
+++ b/Sam's Adventures/Automatizador.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Intel\Desktop\SamsAdventureAssets\Sam's Adventures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samue\OneDrive\Documentos\SamsAdventureAssets\Sam's Adventures\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2FC8737-3F20-4A4F-AD0B-351B7409099E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="11100"/>
+    <workbookView xWindow="-17355" yWindow="1470" windowWidth="9375" windowHeight="7500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -119,13 +120,13 @@
     <t>000</t>
   </si>
   <si>
-    <t>0_Fallen_Angels_Slashing_</t>
+    <t>0_Fallen_Angels_Run Slashing_</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -437,27 +438,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
-    <col min="3" max="3" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.44140625" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" customWidth="1"/>
+    <col min="3" max="3" width="32.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C1" t="str">
         <f t="shared" ref="C1:C32" si="0">A1&amp;B1</f>
         <v/>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -466,10 +467,10 @@
       </c>
       <c r="C2" t="str">
         <f t="shared" si="0"/>
-        <v>0_Fallen_Angels_Slashing_000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0_Fallen_Angels_Run Slashing_000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -478,10 +479,10 @@
       </c>
       <c r="C3" t="str">
         <f t="shared" si="0"/>
-        <v>0_Fallen_Angels_Slashing_001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0_Fallen_Angels_Run Slashing_001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -490,10 +491,10 @@
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
-        <v>0_Fallen_Angels_Slashing_002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0_Fallen_Angels_Run Slashing_002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -502,10 +503,10 @@
       </c>
       <c r="C5" t="str">
         <f>A5&amp;B5</f>
-        <v>0_Fallen_Angels_Slashing_003</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0_Fallen_Angels_Run Slashing_003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -514,10 +515,10 @@
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
-        <v>0_Fallen_Angels_Slashing_004</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0_Fallen_Angels_Run Slashing_004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -526,10 +527,10 @@
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
-        <v>0_Fallen_Angels_Slashing_005</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0_Fallen_Angels_Run Slashing_005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -538,10 +539,10 @@
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
-        <v>0_Fallen_Angels_Slashing_006</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0_Fallen_Angels_Run Slashing_006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -550,10 +551,10 @@
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
-        <v>0_Fallen_Angels_Slashing_007</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0_Fallen_Angels_Run Slashing_007</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -562,10 +563,10 @@
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
-        <v>0_Fallen_Angels_Slashing_008</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0_Fallen_Angels_Run Slashing_008</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -574,10 +575,10 @@
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
-        <v>0_Fallen_Angels_Slashing_009</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0_Fallen_Angels_Run Slashing_009</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -586,10 +587,10 @@
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
-        <v>0_Fallen_Angels_Slashing_010</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0_Fallen_Angels_Run Slashing_010</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -597,11 +598,11 @@
         <v>10</v>
       </c>
       <c r="C13" t="str">
-        <f t="shared" si="0"/>
-        <v>0_Fallen_Angels_Slashing_011</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <f>A13&amp;B13</f>
+        <v>0_Fallen_Angels_Run Slashing_011</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -610,10 +611,10 @@
       </c>
       <c r="C14" t="str">
         <f>A14&amp;B14</f>
-        <v>0_Fallen_Angels_Slashing_012</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0_Fallen_Angels_Run Slashing_012</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -622,10 +623,10 @@
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
-        <v>0_Fallen_Angels_Slashing_013</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0_Fallen_Angels_Run Slashing_013</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -634,10 +635,10 @@
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
-        <v>0_Fallen_Angels_Slashing_014</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0_Fallen_Angels_Run Slashing_014</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -646,10 +647,10 @@
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
-        <v>0_Fallen_Angels_Slashing_015</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0_Fallen_Angels_Run Slashing_015</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -658,10 +659,10 @@
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
-        <v>0_Fallen_Angels_Slashing_016</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0_Fallen_Angels_Run Slashing_016</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -670,10 +671,10 @@
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
-        <v>0_Fallen_Angels_Slashing_017</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0_Fallen_Angels_Run Slashing_017</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -682,10 +683,10 @@
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
-        <v>0_Fallen_Angels_Slashing_018</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0_Fallen_Angels_Run Slashing_018</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -694,10 +695,10 @@
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
-        <v>0_Fallen_Angels_Slashing_019</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0_Fallen_Angels_Run Slashing_019</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -706,10 +707,10 @@
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
-        <v>0_Fallen_Angels_Slashing_020</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0_Fallen_Angels_Run Slashing_020</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -718,10 +719,10 @@
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
-        <v>0_Fallen_Angels_Slashing_021</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0_Fallen_Angels_Run Slashing_021</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -730,10 +731,10 @@
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
-        <v>0_Fallen_Angels_Slashing_022</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0_Fallen_Angels_Run Slashing_022</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -742,10 +743,10 @@
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
-        <v>0_Fallen_Angels_Slashing_023</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0_Fallen_Angels_Run Slashing_023</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -754,10 +755,10 @@
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
-        <v>0_Fallen_Angels_Slashing_024</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0_Fallen_Angels_Run Slashing_024</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -766,10 +767,10 @@
       </c>
       <c r="C27" t="str">
         <f t="shared" si="0"/>
-        <v>0_Fallen_Angels_Slashing_025</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0_Fallen_Angels_Run Slashing_025</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -778,10 +779,10 @@
       </c>
       <c r="C28" t="str">
         <f t="shared" si="0"/>
-        <v>0_Fallen_Angels_Slashing_026</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0_Fallen_Angels_Run Slashing_026</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -790,10 +791,10 @@
       </c>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
-        <v>0_Fallen_Angels_Slashing_027</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0_Fallen_Angels_Run Slashing_027</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -802,10 +803,10 @@
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
-        <v>0_Fallen_Angels_Slashing_028</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0_Fallen_Angels_Run Slashing_028</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -814,10 +815,10 @@
       </c>
       <c r="C31" t="str">
         <f t="shared" si="0"/>
-        <v>0_Fallen_Angels_Slashing_029</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0_Fallen_Angels_Run Slashing_029</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -826,7 +827,7 @@
       </c>
       <c r="C32" t="str">
         <f t="shared" si="0"/>
-        <v>0_Fallen_Angels_Slashing_030</v>
+        <v>0_Fallen_Angels_Run Slashing_030</v>
       </c>
     </row>
   </sheetData>

</xml_diff>